<commit_message>
New additions to extracted data
</commit_message>
<xml_diff>
--- a/data-raw/IDEAIS_4.5-6_fase3-extracciondatos.xlsx
+++ b/data-raw/IDEAIS_4.5-6_fase3-extracciondatos.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="389">
   <si>
     <t>PLANTILLA DE EXTRACCIÓN DE DATOS</t>
   </si>
@@ -137,7 +137,7 @@
     <t>SpaceBook</t>
   </si>
   <si>
-    <t>Edimburgo (UK)</t>
+    <t>Edimburgo, UK</t>
   </si>
   <si>
     <t>mobile-based</t>
@@ -293,7 +293,7 @@
     <t>Citicafe: An interactive interface for citizen engagement</t>
   </si>
   <si>
-    <t>Suporte a la ciudadanía para la solución de problemas cívicos en la ciudad</t>
+    <t>Soporte a la ciudadanía para la solución de problemas cívicos en la ciudad</t>
   </si>
   <si>
     <t>CitiCafe</t>
@@ -531,7 +531,7 @@
     <t>Visitas guiadas</t>
   </si>
   <si>
-    <t>Padula Charterhouse “San Lorenzo” (Italy)</t>
+    <t>Padula Charterhouse “San Lorenzo”, Italy</t>
   </si>
   <si>
     <t>Kinect</t>
@@ -641,7 +641,7 @@
 </t>
   </si>
   <si>
-    <t>Oleander, California</t>
+    <t>Oleander, California, USA</t>
   </si>
   <si>
     <t xml:space="preserve">Análisis de datos espaciales
@@ -928,7 +928,7 @@
     <t>Otro de NER- Lo que se decida para "043" y "046", tambien para este</t>
   </si>
   <si>
-    <t>Reconomiento automático del habla para entidades lugar</t>
+    <t>Reconocimiento automático del habla para entidades lugar</t>
   </si>
   <si>
     <t>Knowledge graphs AND Speech recognition AND Entity relation</t>
@@ -974,6 +974,251 @@
   </si>
   <si>
     <t>texto AND mapas</t>
+  </si>
+  <si>
+    <t>049</t>
+  </si>
+  <si>
+    <t>Rosario</t>
+  </si>
+  <si>
+    <t>Kadaster Knowledge Graph: Beyond the Fifth Star of Open Data</t>
+  </si>
+  <si>
+    <t>INFORMATION</t>
+  </si>
+  <si>
+    <t>Chatbot con reconocimiento de localización</t>
+  </si>
+  <si>
+    <t>Loki</t>
+  </si>
+  <si>
+    <t>The Netherlands</t>
+  </si>
+  <si>
+    <t>linked data AND knowledge graph AND semantic enrichment AND location-aware chatbots AND governmental open data</t>
+  </si>
+  <si>
+    <t>Panel de chat con un visor de mapas para acceso a información geoespacial.</t>
+  </si>
+  <si>
+    <t>información de catastro y registro de tierras</t>
+  </si>
+  <si>
+    <t>Chatbot: Plataforma Rasa (Phytom). Reconocimiento voz: API Microsoft. PDOK SPARQL.</t>
+  </si>
+  <si>
+    <t>voz AND texto AND visual</t>
+  </si>
+  <si>
+    <t>selección, distancia, geometrías</t>
+  </si>
+  <si>
+    <t>050</t>
+  </si>
+  <si>
+    <t>Miscommunication Detection and Recovery in Situated Human-Robot Dialogue</t>
+  </si>
+  <si>
+    <t>ACM TRANSACTIONS ON INTERACTIVE INTELLIGENT SYSTEMS</t>
+  </si>
+  <si>
+    <t>Interfaz conversacional entre un operador humano y un equipo de uno o más robots.</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>TeamTalk</t>
+  </si>
+  <si>
+    <t>Human–robot communication AND physically situated dialogue AND spoken-dialogue systems AND language grounding</t>
+  </si>
+  <si>
+    <t>Detección y recuperación de comunicación humano-robot</t>
+  </si>
+  <si>
+    <t>Instrucciones de navegación emitidas por los usuarios</t>
+  </si>
+  <si>
+    <t>Marco de diálogo: Olympus. 
+ Robots virtuales: USARSim.
+ MOAST SIMware: proxy middleware.</t>
+  </si>
+  <si>
+    <t>voz AND texto AND mapa 2D</t>
+  </si>
+  <si>
+    <t>053</t>
+  </si>
+  <si>
+    <t>X MARKS THE BOT: ONLINE CODING-BASED TREASURE HUNT GAMES FOR CODE LITERACY</t>
+  </si>
+  <si>
+    <t>12TH INTERNATIONAL TECHNOLOGY, EDUCATION AND DEVELOPMENT CONFERENCE (INTED)</t>
+  </si>
+  <si>
+    <t>chatbot para juego multijugador</t>
+  </si>
+  <si>
+    <t>treasurehuntbot</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>code literacy AND messaging bot AND mixed reality</t>
+  </si>
+  <si>
+    <t>Promover la código-alfabetización a través de un juego multijugador guiado por un bot de Telegram</t>
+  </si>
+  <si>
+    <t>mapas, instrucciones del juego</t>
+  </si>
+  <si>
+    <t>texto AND QR code</t>
+  </si>
+  <si>
+    <t>texto, mapas</t>
+  </si>
+  <si>
+    <t>054</t>
+  </si>
+  <si>
+    <t>Villie</t>
+  </si>
+  <si>
+    <t>A Framework for Research in Gamified Mobile Guide Applications using Embodied Conversational Agents (ECAs)</t>
+  </si>
+  <si>
+    <t>INTERNATIONAL JOURNAL OF SERIOUS GAMES</t>
+  </si>
+  <si>
+    <t>Gamified Mobile Guide Applications</t>
+  </si>
+  <si>
+    <t>Lancashire, UK</t>
+  </si>
+  <si>
+    <t>Gamification AND Embodied Conversational Agents</t>
+  </si>
+  <si>
+    <t>Mejoramiento de eficiencia para localización basado en gamificación</t>
+  </si>
+  <si>
+    <t>Información de sensores y de persepción del entorno.</t>
+  </si>
+  <si>
+    <t>Estudios experimentales</t>
+  </si>
+  <si>
+    <t>framework</t>
+  </si>
+  <si>
+    <t>056</t>
+  </si>
+  <si>
+    <t>Enhancing Environmental Engagement with Natural Language Interfaces for In-Vehicle Navigation Systems</t>
+  </si>
+  <si>
+    <t>JOURNAL OF NAVIGATION</t>
+  </si>
+  <si>
+    <t>&amp; McCabe’s (1983) adaptation of the Labovian narrative analysis</t>
+  </si>
+  <si>
+    <t>satnav</t>
+  </si>
+  <si>
+    <t>Nottingham, UK</t>
+  </si>
+  <si>
+    <t>SatNav; Informed Passenger; Collaborative Passanger; Natural Language Interface</t>
+  </si>
+  <si>
+    <t>Natural Language Interfaces AND Vehicle Navigation Systems</t>
+  </si>
+  <si>
+    <t>Selección de ruta</t>
+  </si>
+  <si>
+    <t>camaras de video, base de datos, pasajeros colaborativos, activo pasivo</t>
+  </si>
+  <si>
+    <t>Navegación autónoma con información de marcas (hitos, lugares)</t>
+  </si>
+  <si>
+    <t>Imágenes por camara, mapas, colaboradores</t>
+  </si>
+  <si>
+    <t>ruta de manejo</t>
+  </si>
+  <si>
+    <t>057</t>
+  </si>
+  <si>
+    <t>Luis</t>
+  </si>
+  <si>
+    <t>An interactive virtual guide for the AR based visit of archaeological sites</t>
+  </si>
+  <si>
+    <t>Journal of Visual Languages and Computing</t>
+  </si>
+  <si>
+    <t>Archeological sites</t>
+  </si>
+  <si>
+    <t>Augmented reality AND RFID AND Automata</t>
+  </si>
+  <si>
+    <t>A tour to a set of exhibits lcated within a cultural heritage site by means of an avatar</t>
+  </si>
+  <si>
+    <t>Positional/rotational data streams</t>
+  </si>
+  <si>
+    <t>VRML file</t>
+  </si>
+  <si>
+    <t>058</t>
+  </si>
+  <si>
+    <t>An IoT-based mobile gateway for intelligent personal assistants on mobile health environments</t>
+  </si>
+  <si>
+    <t>Journal of Network and Computer Applications</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Implementación-prototipo</t>
+  </si>
+  <si>
+    <t>Portugal, Brazil, Saudi Arabia, and Russia</t>
+  </si>
+  <si>
+    <t>AMBRO</t>
+  </si>
+  <si>
+    <t>IoT AND Cloud</t>
+  </si>
+  <si>
+    <t>To monitor a person in real-time and collects information about his/her environment, collecting localtion and heart rate of the user</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Smartphone GPS</t>
+  </si>
+  <si>
+    <t>coordinates and activity detected</t>
+  </si>
+  <si>
+    <t>visual</t>
   </si>
 </sst>
 </file>
@@ -1058,7 +1303,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="45">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1156,6 +1401,30 @@
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -1391,7 +1660,10 @@
     <pageSetUpPr/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2.0" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B4" sqref="B4" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
@@ -1403,10 +1675,11 @@
     <col customWidth="1" min="6" max="6" width="8.13"/>
     <col customWidth="1" min="7" max="7" width="16.5"/>
     <col customWidth="1" min="8" max="8" width="22.88"/>
-    <col customWidth="1" min="9" max="9" width="16.38"/>
+    <col customWidth="1" min="9" max="9" width="20.25"/>
     <col customWidth="1" min="10" max="10" width="11.63"/>
     <col customWidth="1" min="11" max="11" width="9.25"/>
-    <col customWidth="1" min="12" max="13" width="11.25"/>
+    <col customWidth="1" min="12" max="12" width="30.0"/>
+    <col customWidth="1" min="13" max="13" width="11.25"/>
     <col customWidth="1" min="14" max="14" width="21.75"/>
     <col customWidth="1" min="15" max="15" width="17.5"/>
     <col customWidth="1" min="16" max="16" width="17.0"/>
@@ -1562,7 +1835,7 @@
       <c r="J3" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="18" t="s">
         <v>32</v>
       </c>
       <c r="L3" s="17" t="s">
@@ -1572,13 +1845,13 @@
       <c r="N3" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="O3" s="18" t="s">
+      <c r="O3" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="P3" s="18" t="s">
+      <c r="P3" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="Q3" s="18" t="s">
+      <c r="Q3" s="17" t="s">
         <v>37</v>
       </c>
       <c r="R3" s="17" t="s">
@@ -1733,7 +2006,7 @@
       <c r="G6" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="17" t="s">
         <v>65</v>
       </c>
       <c r="I6" s="17" t="s">
@@ -1754,7 +2027,7 @@
         <v>68</v>
       </c>
       <c r="P6" s="17"/>
-      <c r="Q6" s="18" t="s">
+      <c r="Q6" s="17" t="s">
         <v>69</v>
       </c>
       <c r="R6" s="17" t="s">
@@ -1851,7 +2124,7 @@
         <v>28</v>
       </c>
       <c r="G8" s="16"/>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="17" t="s">
         <v>84</v>
       </c>
       <c r="I8" s="17" t="s">
@@ -1870,7 +2143,7 @@
       <c r="N8" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="O8" s="18" t="s">
+      <c r="O8" s="17" t="s">
         <v>89</v>
       </c>
       <c r="P8" s="22"/>
@@ -1878,7 +2151,7 @@
       <c r="R8" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="S8" s="18" t="s">
+      <c r="S8" s="17" t="s">
         <v>90</v>
       </c>
       <c r="T8" s="17" t="s">
@@ -1911,7 +2184,7 @@
         <v>28</v>
       </c>
       <c r="G9" s="16"/>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="17" t="s">
         <v>96</v>
       </c>
       <c r="I9" s="17" t="s">
@@ -1927,13 +2200,13 @@
       <c r="M9" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="N9" s="18" t="s">
+      <c r="N9" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="O9" s="18" t="s">
+      <c r="O9" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="P9" s="18" t="s">
+      <c r="P9" s="17" t="s">
         <v>102</v>
       </c>
       <c r="Q9" s="22"/>
@@ -1971,7 +2244,7 @@
       <c r="G10" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="17" t="s">
         <v>108</v>
       </c>
       <c r="I10" s="17" t="s">
@@ -1984,23 +2257,23 @@
       <c r="L10" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="M10" s="18" t="s">
+      <c r="M10" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="N10" s="18" t="s">
+      <c r="N10" s="17" t="s">
         <v>111</v>
       </c>
       <c r="O10" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="P10" s="18" t="s">
+      <c r="P10" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="Q10" s="18"/>
+      <c r="Q10" s="17"/>
       <c r="R10" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="S10" s="18" t="s">
+      <c r="S10" s="17" t="s">
         <v>114</v>
       </c>
       <c r="T10" s="17" t="s">
@@ -2031,7 +2304,7 @@
       <c r="G11" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="17" t="s">
         <v>118</v>
       </c>
       <c r="I11" s="17" t="s">
@@ -2047,13 +2320,13 @@
       <c r="M11" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="N11" s="18" t="s">
+      <c r="N11" s="17" t="s">
         <v>121</v>
       </c>
       <c r="O11" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="P11" s="18" t="s">
+      <c r="P11" s="17" t="s">
         <v>123</v>
       </c>
       <c r="Q11" s="22"/>
@@ -2069,7 +2342,7 @@
       <c r="U11" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="V11" s="18"/>
+      <c r="V11" s="17"/>
     </row>
     <row r="12" ht="64.5" customHeight="1">
       <c r="A12" s="11" t="s">
@@ -2091,7 +2364,7 @@
       <c r="G12" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="17" t="s">
         <v>118</v>
       </c>
       <c r="I12" s="17" t="s">
@@ -2107,13 +2380,13 @@
       <c r="M12" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="N12" s="18" t="s">
+      <c r="N12" s="17" t="s">
         <v>121</v>
       </c>
       <c r="O12" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="P12" s="18" t="s">
+      <c r="P12" s="17" t="s">
         <v>129</v>
       </c>
       <c r="Q12" s="22"/>
@@ -2151,7 +2424,7 @@
       <c r="G13" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="H13" s="18" t="s">
+      <c r="H13" s="17" t="s">
         <v>29</v>
       </c>
       <c r="I13" s="17" t="s">
@@ -2169,7 +2442,7 @@
       <c r="O13" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="P13" s="18" t="s">
+      <c r="P13" s="17" t="s">
         <v>136</v>
       </c>
       <c r="Q13" s="22"/>
@@ -2326,7 +2599,7 @@
         <v>47</v>
       </c>
       <c r="J16" s="22"/>
-      <c r="K16" s="17" t="s">
+      <c r="K16" s="18" t="s">
         <v>161</v>
       </c>
       <c r="L16" s="17" t="s">
@@ -2338,13 +2611,13 @@
       <c r="N16" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="O16" s="18" t="s">
+      <c r="O16" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="P16" s="18" t="s">
+      <c r="P16" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="Q16" s="18" t="s">
+      <c r="Q16" s="17" t="s">
         <v>166</v>
       </c>
       <c r="R16" s="17" t="s">
@@ -2383,7 +2656,7 @@
       <c r="G17" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="H17" s="17" t="s">
         <v>171</v>
       </c>
       <c r="I17" s="17" t="s">
@@ -2403,7 +2676,7 @@
       <c r="O17" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="P17" s="18" t="s">
+      <c r="P17" s="17" t="s">
         <v>165</v>
       </c>
       <c r="Q17" s="22"/>
@@ -2439,7 +2712,7 @@
         <v>28</v>
       </c>
       <c r="G18" s="26"/>
-      <c r="H18" s="18" t="s">
+      <c r="H18" s="17" t="s">
         <v>178</v>
       </c>
       <c r="I18" s="17" t="s">
@@ -2466,7 +2739,7 @@
       <c r="T18" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="U18" s="18" t="s">
+      <c r="U18" s="17" t="s">
         <v>137</v>
       </c>
       <c r="V18" s="22"/>
@@ -2489,7 +2762,7 @@
         <v>28</v>
       </c>
       <c r="G19" s="26"/>
-      <c r="H19" s="18" t="s">
+      <c r="H19" s="17" t="s">
         <v>185</v>
       </c>
       <c r="I19" s="17" t="s">
@@ -2512,7 +2785,7 @@
       <c r="P19" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="Q19" s="18" t="s">
+      <c r="Q19" s="17" t="s">
         <v>190</v>
       </c>
       <c r="R19" s="17" t="s">
@@ -2551,7 +2824,7 @@
         <v>28</v>
       </c>
       <c r="G20" s="26"/>
-      <c r="H20" s="18" t="s">
+      <c r="H20" s="17" t="s">
         <v>195</v>
       </c>
       <c r="I20" s="17" t="s">
@@ -2560,20 +2833,20 @@
       <c r="J20" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="K20" s="17" t="s">
+      <c r="K20" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="L20" s="18" t="s">
+      <c r="L20" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="M20" s="18"/>
+      <c r="M20" s="17"/>
       <c r="N20" s="27" t="s">
         <v>187</v>
       </c>
       <c r="O20" s="27" t="s">
         <v>198</v>
       </c>
-      <c r="P20" s="18" t="s">
+      <c r="P20" s="17" t="s">
         <v>199</v>
       </c>
       <c r="Q20" s="17" t="s">
@@ -2613,7 +2886,7 @@
         <v>28</v>
       </c>
       <c r="G21" s="26"/>
-      <c r="H21" s="18" t="s">
+      <c r="H21" s="17" t="s">
         <v>206</v>
       </c>
       <c r="I21" s="17" t="s">
@@ -2623,10 +2896,10 @@
       <c r="K21" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="L21" s="18" t="s">
+      <c r="L21" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="M21" s="18"/>
+      <c r="M21" s="17"/>
       <c r="N21" s="17" t="s">
         <v>209</v>
       </c>
@@ -2669,7 +2942,7 @@
         <v>28</v>
       </c>
       <c r="G22" s="26"/>
-      <c r="H22" s="18" t="s">
+      <c r="H22" s="17" t="s">
         <v>214</v>
       </c>
       <c r="I22" s="17" t="s">
@@ -2677,10 +2950,10 @@
       </c>
       <c r="J22" s="22"/>
       <c r="K22" s="22"/>
-      <c r="L22" s="18" t="s">
+      <c r="L22" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="M22" s="18"/>
+      <c r="M22" s="17"/>
       <c r="N22" s="17" t="s">
         <v>209</v>
       </c>
@@ -2729,7 +3002,7 @@
       </c>
       <c r="J23" s="30"/>
       <c r="K23" s="30"/>
-      <c r="L23" s="18" t="s">
+      <c r="L23" s="17" t="s">
         <v>78</v>
       </c>
       <c r="M23" s="29"/>
@@ -2995,7 +3268,7 @@
       <c r="G28" s="20" t="s">
         <v>263</v>
       </c>
-      <c r="H28" s="18" t="s">
+      <c r="H28" s="17" t="s">
         <v>29</v>
       </c>
       <c r="I28" s="17" t="s">
@@ -3007,19 +3280,19 @@
       <c r="K28" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="L28" s="18" t="s">
+      <c r="L28" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="M28" s="18" t="s">
+      <c r="M28" s="17" t="s">
         <v>266</v>
       </c>
       <c r="N28" s="17" t="s">
         <v>267</v>
       </c>
-      <c r="O28" s="18" t="s">
+      <c r="O28" s="17" t="s">
         <v>268</v>
       </c>
-      <c r="P28" s="18" t="s">
+      <c r="P28" s="17" t="s">
         <v>269</v>
       </c>
       <c r="Q28" s="22"/>
@@ -3057,7 +3330,7 @@
       <c r="G29" s="20" t="s">
         <v>273</v>
       </c>
-      <c r="H29" s="18" t="s">
+      <c r="H29" s="17" t="s">
         <v>274</v>
       </c>
       <c r="I29" s="17" t="s">
@@ -3109,7 +3382,7 @@
         <v>28</v>
       </c>
       <c r="G30" s="26"/>
-      <c r="H30" s="18" t="s">
+      <c r="H30" s="17" t="s">
         <v>29</v>
       </c>
       <c r="I30" s="17" t="s">
@@ -3121,17 +3394,17 @@
       <c r="K30" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="L30" s="18" t="s">
+      <c r="L30" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="M30" s="18"/>
+      <c r="M30" s="17"/>
       <c r="N30" s="17" t="s">
         <v>283</v>
       </c>
       <c r="O30" s="17" t="s">
         <v>284</v>
       </c>
-      <c r="P30" s="18" t="s">
+      <c r="P30" s="17" t="s">
         <v>285</v>
       </c>
       <c r="Q30" s="17" t="s">
@@ -3173,7 +3446,7 @@
       <c r="G31" s="20" t="s">
         <v>291</v>
       </c>
-      <c r="H31" s="18" t="s">
+      <c r="H31" s="17" t="s">
         <v>292</v>
       </c>
       <c r="I31" s="17" t="s">
@@ -3190,7 +3463,7 @@
       <c r="N31" s="17" t="s">
         <v>293</v>
       </c>
-      <c r="O31" s="18" t="s">
+      <c r="O31" s="17" t="s">
         <v>294</v>
       </c>
       <c r="P31" s="17" t="s">
@@ -3233,7 +3506,7 @@
       <c r="G32" s="15" t="s">
         <v>299</v>
       </c>
-      <c r="H32" s="18" t="s">
+      <c r="H32" s="17" t="s">
         <v>300</v>
       </c>
       <c r="I32" s="17" t="s">
@@ -3254,7 +3527,7 @@
       <c r="N32" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="O32" s="18" t="s">
+      <c r="O32" s="17" t="s">
         <v>304</v>
       </c>
       <c r="P32" s="17" t="s">
@@ -3273,28 +3546,482 @@
       <c r="U32" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="V32" s="18"/>
+      <c r="V32" s="17"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="E33" s="21"/>
+      <c r="A33" s="36" t="s">
+        <v>308</v>
+      </c>
+      <c r="B33" s="37" t="s">
+        <v>309</v>
+      </c>
+      <c r="C33" s="38">
+        <v>2019.0</v>
+      </c>
+      <c r="D33" s="37" t="s">
+        <v>310</v>
+      </c>
+      <c r="E33" s="37" t="s">
+        <v>311</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G33" s="39"/>
+      <c r="H33" s="28" t="s">
+        <v>312</v>
+      </c>
+      <c r="I33" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J33" s="28" t="s">
+        <v>313</v>
+      </c>
+      <c r="K33" s="28" t="s">
+        <v>314</v>
+      </c>
+      <c r="L33" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="M33" s="40"/>
+      <c r="N33" s="28" t="s">
+        <v>315</v>
+      </c>
+      <c r="O33" s="28" t="s">
+        <v>316</v>
+      </c>
+      <c r="P33" s="28" t="s">
+        <v>317</v>
+      </c>
+      <c r="Q33" s="28" t="s">
+        <v>318</v>
+      </c>
+      <c r="R33" s="28" t="s">
+        <v>319</v>
+      </c>
+      <c r="S33" s="28" t="s">
+        <v>307</v>
+      </c>
+      <c r="T33" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="U33" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="V33" s="28" t="s">
+        <v>320</v>
+      </c>
+      <c r="W33" s="39"/>
+      <c r="X33" s="39"/>
+      <c r="Y33" s="39"/>
+      <c r="Z33" s="39"/>
+      <c r="AA33" s="39"/>
+      <c r="AB33" s="39"/>
+      <c r="AC33" s="39"/>
+      <c r="AD33" s="39"/>
+      <c r="AE33" s="39"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
-      <c r="E34" s="21"/>
+      <c r="A34" s="36" t="s">
+        <v>321</v>
+      </c>
+      <c r="B34" s="37" t="s">
+        <v>309</v>
+      </c>
+      <c r="C34" s="38">
+        <v>2019.0</v>
+      </c>
+      <c r="D34" s="37" t="s">
+        <v>322</v>
+      </c>
+      <c r="E34" s="37" t="s">
+        <v>323</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G34" s="39"/>
+      <c r="H34" s="28" t="s">
+        <v>324</v>
+      </c>
+      <c r="I34" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="J34" s="40"/>
+      <c r="K34" s="28" t="s">
+        <v>325</v>
+      </c>
+      <c r="L34" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="M34" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="N34" s="28" t="s">
+        <v>327</v>
+      </c>
+      <c r="O34" s="28" t="s">
+        <v>328</v>
+      </c>
+      <c r="P34" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q34" s="28" t="s">
+        <v>330</v>
+      </c>
+      <c r="R34" s="28" t="s">
+        <v>259</v>
+      </c>
+      <c r="S34" s="28" t="s">
+        <v>331</v>
+      </c>
+      <c r="T34" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="U34" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="V34" s="41"/>
+      <c r="W34" s="39"/>
+      <c r="X34" s="39"/>
+      <c r="Y34" s="39"/>
+      <c r="Z34" s="39"/>
+      <c r="AA34" s="39"/>
+      <c r="AB34" s="39"/>
+      <c r="AC34" s="39"/>
+      <c r="AD34" s="39"/>
+      <c r="AE34" s="39"/>
     </row>
     <row r="35" ht="14.25" customHeight="1">
-      <c r="E35" s="21"/>
+      <c r="A35" s="36" t="s">
+        <v>332</v>
+      </c>
+      <c r="B35" s="37" t="s">
+        <v>309</v>
+      </c>
+      <c r="C35" s="38">
+        <v>2018.0</v>
+      </c>
+      <c r="D35" s="37" t="s">
+        <v>333</v>
+      </c>
+      <c r="E35" s="37" t="s">
+        <v>334</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G35" s="39"/>
+      <c r="H35" s="28" t="s">
+        <v>335</v>
+      </c>
+      <c r="I35" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J35" s="28" t="s">
+        <v>336</v>
+      </c>
+      <c r="K35" s="28" t="s">
+        <v>337</v>
+      </c>
+      <c r="L35" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="M35" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="N35" s="28" t="s">
+        <v>338</v>
+      </c>
+      <c r="O35" s="28" t="s">
+        <v>339</v>
+      </c>
+      <c r="P35" s="28" t="s">
+        <v>340</v>
+      </c>
+      <c r="Q35" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="R35" s="28" t="s">
+        <v>341</v>
+      </c>
+      <c r="S35" s="28" t="s">
+        <v>342</v>
+      </c>
+      <c r="T35" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="U35" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="V35" s="41"/>
+      <c r="W35" s="39"/>
+      <c r="X35" s="39"/>
+      <c r="Y35" s="39"/>
+      <c r="Z35" s="39"/>
+      <c r="AA35" s="39"/>
+      <c r="AB35" s="39"/>
+      <c r="AC35" s="39"/>
+      <c r="AD35" s="39"/>
+      <c r="AE35" s="39"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
-      <c r="E36" s="21"/>
+      <c r="A36" s="36" t="s">
+        <v>343</v>
+      </c>
+      <c r="B36" s="37" t="s">
+        <v>344</v>
+      </c>
+      <c r="C36" s="42">
+        <v>2015.0</v>
+      </c>
+      <c r="D36" s="37" t="s">
+        <v>345</v>
+      </c>
+      <c r="E36" s="43" t="s">
+        <v>346</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G36" s="39"/>
+      <c r="H36" s="28" t="s">
+        <v>347</v>
+      </c>
+      <c r="I36" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="J36" s="40"/>
+      <c r="K36" s="28" t="s">
+        <v>348</v>
+      </c>
+      <c r="L36" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="M36" s="28"/>
+      <c r="N36" s="28" t="s">
+        <v>349</v>
+      </c>
+      <c r="O36" s="28" t="s">
+        <v>350</v>
+      </c>
+      <c r="P36" s="28" t="s">
+        <v>351</v>
+      </c>
+      <c r="Q36" s="40"/>
+      <c r="R36" s="28" t="s">
+        <v>352</v>
+      </c>
+      <c r="S36" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="T36" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="U36" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="V36" s="41"/>
+      <c r="W36" s="39"/>
+      <c r="X36" s="39"/>
+      <c r="Y36" s="39"/>
+      <c r="Z36" s="39"/>
+      <c r="AA36" s="39"/>
+      <c r="AB36" s="39"/>
+      <c r="AC36" s="39"/>
+      <c r="AD36" s="39"/>
+      <c r="AE36" s="39"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
-      <c r="E37" s="21"/>
+      <c r="A37" s="36" t="s">
+        <v>354</v>
+      </c>
+      <c r="B37" s="37" t="s">
+        <v>344</v>
+      </c>
+      <c r="C37" s="42">
+        <v>2019.0</v>
+      </c>
+      <c r="D37" s="37" t="s">
+        <v>355</v>
+      </c>
+      <c r="E37" s="43" t="s">
+        <v>356</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G37" s="39"/>
+      <c r="H37" s="28" t="s">
+        <v>357</v>
+      </c>
+      <c r="I37" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="J37" s="28" t="s">
+        <v>358</v>
+      </c>
+      <c r="K37" s="28" t="s">
+        <v>359</v>
+      </c>
+      <c r="L37" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="M37" s="28" t="s">
+        <v>360</v>
+      </c>
+      <c r="N37" s="28" t="s">
+        <v>361</v>
+      </c>
+      <c r="O37" s="28" t="s">
+        <v>362</v>
+      </c>
+      <c r="P37" s="28" t="s">
+        <v>363</v>
+      </c>
+      <c r="Q37" s="28" t="s">
+        <v>364</v>
+      </c>
+      <c r="R37" s="28" t="s">
+        <v>365</v>
+      </c>
+      <c r="S37" s="28" t="s">
+        <v>366</v>
+      </c>
+      <c r="T37" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="U37" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="V37" s="28" t="s">
+        <v>362</v>
+      </c>
+      <c r="W37" s="39"/>
+      <c r="X37" s="39"/>
+      <c r="Y37" s="39"/>
+      <c r="Z37" s="39"/>
+      <c r="AA37" s="39"/>
+      <c r="AB37" s="39"/>
+      <c r="AC37" s="39"/>
+      <c r="AD37" s="39"/>
+      <c r="AE37" s="39"/>
     </row>
     <row r="38" ht="14.25" customHeight="1">
-      <c r="E38" s="21"/>
+      <c r="A38" s="36" t="s">
+        <v>367</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>368</v>
+      </c>
+      <c r="C38" s="15">
+        <v>2011.0</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>369</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>370</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H38" s="44" t="s">
+        <v>371</v>
+      </c>
+      <c r="I38" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="J38" s="44"/>
+      <c r="K38" s="44" t="s">
+        <v>337</v>
+      </c>
+      <c r="L38" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M38" s="44"/>
+      <c r="N38" s="44" t="s">
+        <v>372</v>
+      </c>
+      <c r="O38" s="44" t="s">
+        <v>373</v>
+      </c>
+      <c r="P38" s="44" t="s">
+        <v>374</v>
+      </c>
+      <c r="Q38" s="44" t="s">
+        <v>375</v>
+      </c>
+      <c r="R38" s="24"/>
+      <c r="S38" s="24"/>
+      <c r="T38" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="U38" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="V38" s="24"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
-      <c r="E39" s="21"/>
+      <c r="A39" s="36" t="s">
+        <v>376</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>368</v>
+      </c>
+      <c r="C39" s="15">
+        <v>2016.0</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>377</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>378</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H39" s="44" t="s">
+        <v>379</v>
+      </c>
+      <c r="I39" s="44" t="s">
+        <v>380</v>
+      </c>
+      <c r="J39" s="44"/>
+      <c r="K39" s="44" t="s">
+        <v>381</v>
+      </c>
+      <c r="L39" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M39" s="44" t="s">
+        <v>382</v>
+      </c>
+      <c r="N39" s="44" t="s">
+        <v>383</v>
+      </c>
+      <c r="O39" s="44" t="s">
+        <v>384</v>
+      </c>
+      <c r="P39" s="44" t="s">
+        <v>385</v>
+      </c>
+      <c r="Q39" s="44" t="s">
+        <v>386</v>
+      </c>
+      <c r="R39" s="44" t="s">
+        <v>387</v>
+      </c>
+      <c r="S39" s="44" t="s">
+        <v>388</v>
+      </c>
+      <c r="T39" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="U39" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="V39" s="24"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="E40" s="21"/>
@@ -5759,16 +6486,16 @@
     <row r="860" ht="14.25" customHeight="1">
       <c r="E860" s="21"/>
     </row>
-    <row r="861">
+    <row r="861" ht="14.25" customHeight="1">
       <c r="E861" s="21"/>
     </row>
-    <row r="862">
+    <row r="862" ht="14.25" customHeight="1">
       <c r="E862" s="21"/>
     </row>
-    <row r="863">
+    <row r="863" ht="14.25" customHeight="1">
       <c r="E863" s="21"/>
     </row>
-    <row r="864">
+    <row r="864" ht="14.25" customHeight="1">
       <c r="E864" s="21"/>
     </row>
     <row r="865">
@@ -6125,13 +6852,25 @@
     <row r="982">
       <c r="E982" s="21"/>
     </row>
+    <row r="983">
+      <c r="E983" s="21"/>
+    </row>
+    <row r="984">
+      <c r="E984" s="21"/>
+    </row>
+    <row r="985">
+      <c r="E985" s="21"/>
+    </row>
+    <row r="986">
+      <c r="E986" s="21"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F3:F32">
+  <conditionalFormatting sqref="F3:F39">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$F3="S"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F32">
+  <conditionalFormatting sqref="F3:F39">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>$F3="N"</formula>
     </cfRule>

</xml_diff>